<commit_message>
Update midterm and HW1
</commit_message>
<xml_diff>
--- a/data/multi_asset_etf_data.xlsx
+++ b/data/multi_asset_etf_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shenchingfeng/Desktop/FinMath/Autumn/Portfolio and Risk Management/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shenchingfeng/Documents/FinMath/Autumn/Portfolio and Risk Management/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F100D25-6E18-3447-8DA2-3FBD60FC3CD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845DD0CF-88B7-1A4E-8393-1477129F27D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="29400" windowHeight="18460" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="29400" windowHeight="18460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="descriptions" sheetId="5" r:id="rId1"/>
@@ -532,13 +532,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0548E9F-AA47-3B46-B903-B92960E1DD5C}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView zoomScale="136" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScale="230" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="28" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -7996,7 +7998,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M173"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>

</xml_diff>